<commit_message>
MALS-224 Unmerge header label cells
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/LicenceType_Location_Template.xlsx
+++ b/app/server/static/templates/reports/LicenceType_Location_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://parcsystems.sharepoint.com/projects/Shared Documents/MALS/CDOGS/Development/MALS_Templates/Reports/Location_Licence_Type/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{BC9164F5-7F50-4B1D-BF60-692053187AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3AB50D2D-7846-ED41-AC44-8B0525BCE5EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D381F535-C512-4FC0-B4F7-14AC229B4660}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="720" windowWidth="23260" windowHeight="12580" xr2:uid="{2E2F7D45-7862-45BB-AE8B-54A6535F5203}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E2F7D45-7862-45BB-AE8B-54A6535F5203}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,26 +185,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,43 +560,43 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="20.5" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
         <v>14</v>
@@ -567,16 +604,16 @@
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
@@ -594,17 +631,17 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -645,27 +682,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="C1:C2"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fc8a81a77eeb73bda9729b3f784b8c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88ad40c7f0e134defa4acd5e486d3459" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -876,12 +913,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -892,6 +923,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A680627D-FEBC-4CFE-869B-A9C927EB5363}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{116685B2-35BD-4ECE-A739-3CFD64521F0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -910,23 +958,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A680627D-FEBC-4CFE-869B-A9C927EB5363}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22953A0A-06BB-4B72-A85C-61108B2DEB25}">
   <ds:schemaRefs>

</xml_diff>